<commit_message>
feat: first version for automatic draft activation
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/ListReportOrdersNoErros.xlsx
+++ b/examples/test/testFiles/ListReportOrdersNoErros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1DCDBE0-086D-904B-AED3-B661D1210644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F59417C-222A-494E-AC4B-9D2AB9FAEB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Created On</t>
   </si>
@@ -434,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -486,11 +486,20 @@
       </c>
       <c r="G2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{6AEF1AA3-6607-0146-ACD9-86E0F0D4AEFD}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{793DD381-A950-4C61-8CB5-912E2AB30FF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
fix: remove columns in list report test file
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/ListReportOrdersNoErros.xlsx
+++ b/examples/test/testFiles/ListReportOrdersNoErros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F59417C-222A-494E-AC4B-9D2AB9FAEB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F385410-B344-7943-8848-D14F302CE4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,30 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
-  <si>
-    <t>Created On</t>
-  </si>
-  <si>
-    <t>Created By</t>
-  </si>
-  <si>
-    <t>Changed On</t>
-  </si>
-  <si>
-    <t>Changed By</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Order Number</t>
   </si>
   <si>
     <t>User ID</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>test@test.de</t>
@@ -434,76 +416,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{6AEF1AA3-6607-0146-ACD9-86E0F0D4AEFD}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{793DD381-A950-4C61-8CB5-912E2AB30FF2}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6AEF1AA3-6607-0146-ACD9-86E0F0D4AEFD}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{793DD381-A950-4C61-8CB5-912E2AB30FF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1 A2:D2 G2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: check if all columns name in file match metadata (#57)
* feat: check if all columns name in file match metadata

Checks on upload if all column names match the corresponding metadata model
Closes #29

* fix: remove columns in list report test file
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/ListReportOrdersNoErros.xlsx
+++ b/examples/test/testFiles/ListReportOrdersNoErros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F59417C-222A-494E-AC4B-9D2AB9FAEB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F385410-B344-7943-8848-D14F302CE4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,30 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
-  <si>
-    <t>Created On</t>
-  </si>
-  <si>
-    <t>Created By</t>
-  </si>
-  <si>
-    <t>Changed On</t>
-  </si>
-  <si>
-    <t>Changed By</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Order Number</t>
   </si>
   <si>
     <t>User ID</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>test@test.de</t>
@@ -434,76 +416,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{6AEF1AA3-6607-0146-ACD9-86E0F0D4AEFD}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{793DD381-A950-4C61-8CB5-912E2AB30FF2}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6AEF1AA3-6607-0146-ACD9-86E0F0D4AEFD}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{793DD381-A950-4C61-8CB5-912E2AB30FF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1 A2:D2 G2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat!: removal of option `fieldMatchType`
new default is `labelTypeBrackets` to avoid any
colisions with labels and types
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/ListReportOrdersNoErros.xlsx
+++ b/examples/test/testFiles/ListReportOrdersNoErros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F385410-B344-7943-8848-D14F302CE4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD8005D-009F-479B-BEA1-257A5349507F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3405" yWindow="1950" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
-    <t>Order Number</t>
+    <t>test@test.de</t>
   </si>
   <si>
-    <t>User ID</t>
+    <t>Order Number[OrderNo]</t>
   </si>
   <si>
-    <t>test@test.de</t>
+    <t>User ID[buyer]</t>
   </si>
 </sst>
 </file>
@@ -419,33 +419,33 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -454,8 +454,5 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{793DD381-A950-4C61-8CB5-912E2AB30FF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:B1" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat!: removal of option `fieldMatchType` (#157)
* feat!: removal of option `fieldMatchType`

new default is `labelTypeBrackets` to avoid any
colisions with labels and types

* test: fix file names

* chore: fix example apps events
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/ListReportOrdersNoErros.xlsx
+++ b/examples/test/testFiles/ListReportOrdersNoErros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F385410-B344-7943-8848-D14F302CE4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD8005D-009F-479B-BEA1-257A5349507F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3405" yWindow="1950" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
-    <t>Order Number</t>
+    <t>test@test.de</t>
   </si>
   <si>
-    <t>User ID</t>
+    <t>Order Number[OrderNo]</t>
   </si>
   <si>
-    <t>test@test.de</t>
+    <t>User ID[buyer]</t>
   </si>
 </sst>
 </file>
@@ -419,33 +419,33 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -454,8 +454,5 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{793DD381-A950-4C61-8CB5-912E2AB30FF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:B1" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test: make 120 new default
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/ListReportOrdersNoErros.xlsx
+++ b/examples/test/testFiles/ListReportOrdersNoErros.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD8005D-009F-479B-BEA1-257A5349507F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE12BFA2-0CC9-F54B-9CEB-B31C3897199E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1950" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3400" yWindow="1960" windowWidth="21600" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>test@test.de</t>
   </si>
@@ -29,6 +30,24 @@
   </si>
   <si>
     <t>User ID[buyer]</t>
+  </si>
+  <si>
+    <t>Test Spalte</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>TEST Spalte</t>
+  </si>
+  <si>
+    <t>tsdf</t>
+  </si>
+  <si>
+    <t>tsdfg</t>
   </si>
 </sst>
 </file>
@@ -416,36 +435,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -455,4 +483,56 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4889AB16-078F-964F-81F8-53346C7B98D5}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CD8D3721-59F3-7847-B373-A1644A218DA6}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{2BB2366D-DE1D-0A4C-9124-1186B0C0CC07}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test: add sample apps for UI5 1.120 (#412)
* test: add test for UI5 1.120

* test: make 120 new default

* test: make 120 default

* fix: port script

* delete app from cap

* fix test excel

* fix: testapps.json

* fix: escape unicode

* fix: testappsjson

* fix: update testapps.json

* fix: update

* test:fix

* fix: exclude 120 wdi5 test
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/ListReportOrdersNoErros.xlsx
+++ b/examples/test/testFiles/ListReportOrdersNoErros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD8005D-009F-479B-BEA1-257A5349507F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEACC664-98E1-D047-86E0-F651498478EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1950" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3400" yWindow="1960" windowWidth="21600" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -419,12 +419,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -432,7 +432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -440,7 +440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
fix: column names did not parse if cell type is date
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/ListReportOrdersNoErros.xlsx
+++ b/examples/test/testFiles/ListReportOrdersNoErros.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-spreadsheetimporter/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEACC664-98E1-D047-86E0-F651498478EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7924575D-68AB-8C41-BB60-FD87A570D11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3400" yWindow="1960" windowWidth="21600" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -419,7 +420,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,7 +429,7 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: column names did not parse if cell type is date (#677)
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/ListReportOrdersNoErros.xlsx
+++ b/examples/test/testFiles/ListReportOrdersNoErros.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-spreadsheetimporter/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEACC664-98E1-D047-86E0-F651498478EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7924575D-68AB-8C41-BB60-FD87A570D11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3400" yWindow="1960" windowWidth="21600" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -419,7 +420,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,7 +429,7 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>